<commit_message>
Added test for integer conversion
</commit_message>
<xml_diff>
--- a/ExcelUtilitiesTests/TestFiles/FirstTest.xlsx
+++ b/ExcelUtilitiesTests/TestFiles/FirstTest.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26925"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="109" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6931558D-48F7-452B-B444-9376FEB6734E}"/>
+  <xr:revisionPtr revIDLastSave="110" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AB2B478-22F6-463A-8A19-058901FF2BC5}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmptyWorksheet" sheetId="5" r:id="rId1"/>
@@ -518,7 +518,7 @@
   <dimension ref="A3:K21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -550,7 +550,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F61C534B-F8A4-4CE8-83F3-7344D7427310}">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -637,10 +637,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7130D372-8F92-4AC3-BF9C-73D8ADAAD97D}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -652,7 +652,7 @@
     <col min="7" max="7" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -674,18 +674,21 @@
       <c r="G1" s="7">
         <v>12.23</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
+      <c r="H1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
       <c r="D2" s="3"/>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8">
       <c r="B3" s="1"/>
       <c r="C3" s="2"/>
       <c r="D3" s="3"/>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:8">
       <c r="E5"/>
       <c r="F5"/>
       <c r="G5"/>

</xml_diff>

<commit_message>
Swapped ClosedXML for Slyvan.Data.Excel to significantly reduce memory consumption and increase speed.
</commit_message>
<xml_diff>
--- a/ExcelUtilitiesTests/TestFiles/FirstTest.xlsx
+++ b/ExcelUtilitiesTests/TestFiles/FirstTest.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27002"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="110" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AB2B478-22F6-463A-8A19-058901FF2BC5}"/>
+  <xr:revisionPtr revIDLastSave="117" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{550CD94F-3E03-4FA8-AE86-2BB5D888F1C3}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmptyWorksheet" sheetId="5" r:id="rId1"/>
@@ -18,6 +18,9 @@
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
   <si>
     <t>First Column</t>
   </si>
@@ -52,9 +55,6 @@
   </si>
   <si>
     <t>one</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>two</t>
@@ -455,7 +455,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:XFD4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -515,10 +515,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9B715B-7741-449B-A1EE-6B1BB3FF1265}">
-  <dimension ref="A3:K21"/>
+  <dimension ref="A3:A4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -533,12 +533,7 @@
     </row>
     <row r="4" spans="1:1">
       <c r="A4" s="8">
-        <v>234</v>
-      </c>
-    </row>
-    <row r="21" spans="11:11">
-      <c r="K21" t="s">
-        <v>6</v>
+        <v>1234</v>
       </c>
     </row>
   </sheetData>
@@ -569,7 +564,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -577,7 +572,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -585,7 +580,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -593,7 +588,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -615,7 +610,7 @@
   <sheetData>
     <row r="1" spans="2:4">
       <c r="B1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -639,7 +634,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7130D372-8F92-4AC3-BF9C-73D8ADAAD97D}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
@@ -713,7 +708,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="30.75">
       <c r="A1" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved test coverage to ensure all code is actually necessary
</commit_message>
<xml_diff>
--- a/ExcelUtilitiesTests/TestFiles/FirstTest.xlsx
+++ b/ExcelUtilitiesTests/TestFiles/FirstTest.xlsx
@@ -3,18 +3,19 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27002"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="117" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{550CD94F-3E03-4FA8-AE86-2BB5D888F1C3}"/>
+  <xr:revisionPtr revIDLastSave="126" documentId="11_E60897F41BE170836B02CE998F75CCDC64E183C8" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E201A3D4-3B6E-47F5-9263-C9F2404BF536}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="5" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" firstSheet="2" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="EmptyWorksheet" sheetId="5" r:id="rId1"/>
     <sheet name="WithHeadings" sheetId="1" r:id="rId2"/>
     <sheet name="HeadingsOnRowThree" sheetId="6" r:id="rId3"/>
     <sheet name="WithBlankRows" sheetId="7" r:id="rId4"/>
-    <sheet name="NoHeadings" sheetId="4" r:id="rId5"/>
-    <sheet name="TypeTests" sheetId="3" r:id="rId6"/>
-    <sheet name="WorksheetByClassName" sheetId="2" r:id="rId7"/>
+    <sheet name="MissingRequired" sheetId="8" r:id="rId5"/>
+    <sheet name="NoHeadings" sheetId="4" r:id="rId6"/>
+    <sheet name="TypeTests" sheetId="3" r:id="rId7"/>
+    <sheet name="WorksheetByClassName" sheetId="2" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>First Column</t>
   </si>
@@ -67,6 +68,18 @@
   </si>
   <si>
     <t>six</t>
+  </si>
+  <si>
+    <t>NonOptional</t>
+  </si>
+  <si>
+    <t>Second</t>
+  </si>
+  <si>
+    <t>first</t>
+  </si>
+  <si>
+    <t>second</t>
   </si>
   <si>
     <t>find me</t>
@@ -517,7 +530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC9B715B-7741-449B-A1EE-6B1BB3FF1265}">
   <dimension ref="A3:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -546,7 +559,7 @@
   <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -597,6 +610,53 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F23F1379-A214-4573-B6CE-C686BAB59074}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BC216077-79C3-41B3-9E6E-4982B3117575}">
   <dimension ref="B1:D3"/>
   <sheetViews>
@@ -610,7 +670,7 @@
   <sheetData>
     <row r="1" spans="2:4">
       <c r="B1" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
@@ -630,7 +690,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7130D372-8F92-4AC3-BF9C-73D8ADAAD97D}">
   <dimension ref="A1:H5"/>
   <sheetViews>
@@ -693,7 +753,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{18CFAF84-A096-4AB9-907A-677FC50DD1A0}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -708,7 +768,7 @@
   <sheetData>
     <row r="1" spans="1:1" ht="30.75">
       <c r="A1" s="4" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>